<commit_message>
Small change in Excel file
</commit_message>
<xml_diff>
--- a/dataset_descriptions.xlsx
+++ b/dataset_descriptions.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u979283\OneDrive - Syngenta\Challenges\Challenge 7 _ 2019 Informs\Datasets\Processed Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xavi/Documents/GitHub/Tools-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3AC8492F7955EA405EBBCC76EA0B9187F8D6BE50" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{1D783438-4E62-4F17-AC7C-D4B30FEC4ADD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5658986-08E0-AB40-8D24-C4844AF86DE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="12300" windowHeight="7680" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23820" windowHeight="11240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_descriptions" sheetId="1" r:id="rId1"/>
-    <sheet name="example_submission" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Dataset</t>
   </si>
@@ -272,96 +271,12 @@
   <si>
     <t>Flag for whether hybrid is resistant to heat+drought as you define it in objective #1</t>
   </si>
-  <si>
-    <t>Example submission 1</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>For this submission, H1 is found to be resistant to heat, drought, and heat + drought</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H2 is found to be resistant to heat and drought, but susceptible to heat + drought</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>H3 is found to be susceptible to all stresses</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <t>H4 is found to be resistant to only drought</t>
-  </si>
-  <si>
-    <t>H5</t>
-  </si>
-  <si>
-    <t>H5 is found to be resistant to only heat</t>
-  </si>
-  <si>
-    <t>Example submission 2</t>
-  </si>
-  <si>
-    <t>HEAT_RES_1</t>
-  </si>
-  <si>
-    <t>HEAT_RES_2</t>
-  </si>
-  <si>
-    <t>HEAT_RES_3</t>
-  </si>
-  <si>
-    <t>DROUGHT_RES_1</t>
-  </si>
-  <si>
-    <t>DROUGHT_RES_2</t>
-  </si>
-  <si>
-    <t>DROUGHT_RES_3</t>
-  </si>
-  <si>
-    <t>HEAT_DROUGHT_RES_1</t>
-  </si>
-  <si>
-    <t>HEAT_DROUGHT_RES_2</t>
-  </si>
-  <si>
-    <t>HEAT_DROUGHT_RES_3</t>
-  </si>
-  <si>
-    <t>For this submission, each stress was quantified by 3 different metrics in objective #1</t>
-  </si>
-  <si>
-    <t>The resulting classifications are far more complex, but perhaps more meaningful depending on the definition of each stress metric</t>
-  </si>
-  <si>
-    <t>Example submission 3</t>
-  </si>
-  <si>
-    <t>This is another option for the same results as example 2</t>
-  </si>
-  <si>
-    <t>For each stress type, the overall result is the median of the individual results in example 2 (equal weight for each metric of each type)</t>
-  </si>
-  <si>
-    <t>If you think one metric is more meaningful than another, you may want to weigh it more heavily</t>
-  </si>
-  <si>
-    <t>e.g. HEAT_RES_1 is more meaningful than HEAT_RES_2 and HEAT_RES_3, so create a weighted average with greater impact to HEAT_RES_1</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -419,12 +334,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,23 +616,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A45" sqref="A45:A52"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="90.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="78.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="111.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="90.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="78.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -737,7 +644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -748,7 +655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -756,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -764,7 +671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -775,7 +682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
@@ -783,7 +690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
@@ -791,7 +698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
@@ -799,7 +706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -807,7 +714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
@@ -815,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
@@ -823,7 +730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="85.5">
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
@@ -834,7 +741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
@@ -843,7 +750,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
@@ -852,7 +759,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
@@ -861,7 +768,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
@@ -872,7 +779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
@@ -881,7 +788,7 @@
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
@@ -889,7 +796,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
@@ -897,7 +804,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
@@ -905,7 +812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
@@ -913,7 +820,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>48</v>
       </c>
@@ -921,7 +828,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>50</v>
@@ -930,10 +837,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
@@ -944,7 +851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>53</v>
       </c>
@@ -955,7 +862,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>56</v>
       </c>
@@ -963,7 +870,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>58</v>
       </c>
@@ -971,7 +878,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
         <v>60</v>
       </c>
@@ -979,7 +886,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
         <v>62</v>
       </c>
@@ -987,7 +894,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
@@ -995,7 +902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
@@ -1003,7 +910,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
@@ -1011,7 +918,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
@@ -1022,7 +929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45">
+    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>72</v>
       </c>
@@ -1033,7 +940,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30">
+    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>75</v>
       </c>
@@ -1044,7 +951,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>78</v>
       </c>
@@ -1061,482 +968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="7"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="7"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="M16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26">
-        <f>MEDIAN(B15:D15)</f>
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <f>MEDIAN(E15:G15)</f>
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <f>MEDIAN(H15:J15)</f>
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27">
-        <f t="shared" ref="B27:B30" si="0">MEDIAN(B16:D16)</f>
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <f t="shared" ref="C27:C30" si="1">MEDIAN(E16:G16)</f>
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <f t="shared" ref="D27:D30" si="2">MEDIAN(H16:J16)</f>
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A342FBBECA86824FA53E70EA0AD86B62" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d819d62a6a9605acdf46129402f77d3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d6dd422e-7e04-43fc-a4d3-1dc86e3f2abc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e716c597a9353ff5dcae2c02963ca7f" ns2:_="">
     <xsd:import namespace="d6dd422e-7e04-43fc-a4d3-1dc86e3f2abc"/>
@@ -1694,14 +1126,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A866955C-BA56-4C71-A935-30B72C7A59DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94DAF173-8757-4641-B4E9-973750A4A6DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d6dd422e-7e04-43fc-a4d3-1dc86e3f2abc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B474AE60-549A-4480-9D3D-42581F20B7B3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B474AE60-549A-4480-9D3D-42581F20B7B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94DAF173-8757-4641-B4E9-973750A4A6DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A866955C-BA56-4C71-A935-30B72C7A59DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>